<commit_message>
complete burndown chart for sprint 3
</commit_message>
<xml_diff>
--- a/sprint-backlog/sprint-3/report-sheet.xlsx
+++ b/sprint-backlog/sprint-3/report-sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="plan" sheetId="1" state="visible" r:id="rId2"/>
@@ -130,12 +130,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FF595959"/>
       <name val="Calibri"/>
@@ -145,6 +139,11 @@
       <sz val="9"/>
       <color rgb="FF595959"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -195,7 +194,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -340,7 +339,6 @@
               <a:solidFill>
                 <a:srgbClr val="636363"/>
               </a:solidFill>
-              <a:custDash/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -358,10 +356,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>burndown!$B$2:$G$2</c:f>
+              <c:f>burndown!$B$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
@@ -379,6 +377,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -424,10 +425,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>burndown!$B$3:$G$3</c:f>
+              <c:f>burndown!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
@@ -445,6 +446,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -459,11 +463,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="49053926"/>
-        <c:axId val="14658829"/>
+        <c:axId val="64639371"/>
+        <c:axId val="47710374"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49053926"/>
+        <c:axId val="64639371"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,14 +503,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14658829"/>
+        <c:crossAx val="47710374"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14658829"/>
+        <c:axId val="47710374"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +553,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49053926"/>
+        <c:crossAx val="64639371"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -598,9 +602,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>371160</xdr:colOff>
+      <xdr:colOff>370800</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:rowOff>182520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -609,7 +613,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1685880" y="647640"/>
-        <a:ext cx="9353160" cy="4267080"/>
+        <a:ext cx="9352800" cy="4266720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -849,7 +853,7 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -1061,8 +1065,8 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R14" activeCellId="0" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>